<commit_message>
i260--eit2 suite file update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/analysis_01_simulation_win.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/analysis_01_simulation_win.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syan\Documents\My Received Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="0sngsN6DrFUqmuDZZhkIhd0EivD5xjZ0nj5fkMPZg+GIws2dGdQ895P+5SBGWtagLIQbEIRaHiBSjM2rhskk/Q==" workbookSaltValue="j22CHco5Hi8vlbKkcb9mlg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="6300" windowWidth="28830" windowHeight="6240"/>
+    <workbookView xWindow="-15" yWindow="6300" windowWidth="28830" windowHeight="6240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -22,19 +22,21 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
     <definedName name="Z_16B2C8B3_13FA_43FB_96C1_3763C72619A6_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
     <definedName name="Z_179F0E1F_F6F7_410E_B883_54B8A90BA550_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
+    <definedName name="Z_B9BD6881_07CB_45A2_88EA_37624FD6A1EC_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
     <definedName name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" localSheetId="1" hidden="1">case!$A$2:$AD$2</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
   <customWorkbookViews>
+    <customWorkbookView name="Shawn Yan - Personal View" guid="{B9BD6881-07CB-45A2-88EA-37624FD6A1EC}" mergeInterval="0" personalView="1" xWindow="-1896" yWindow="46" windowWidth="2418" windowHeight="968" activeSheetId="2"/>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
     <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="407">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -1457,6 +1459,27 @@
   </si>
   <si>
     <t>analysis_01_simulation_win</t>
+  </si>
+  <si>
+    <t>002_vhdl_combinat_adder8_Jedi</t>
+  </si>
+  <si>
+    <t>007_vhdl_combinat_decoder2_Jedi</t>
+  </si>
+  <si>
+    <t>013_vhdl_combinat_interupt_Jedi</t>
+  </si>
+  <si>
+    <t>018_vhdl_combinat_tristate1_Jedi</t>
+  </si>
+  <si>
+    <t>053_vhdl_sequentl_latches_Jedi</t>
+  </si>
+  <si>
+    <t>067_vlog_combinat_alu_Jedi</t>
+  </si>
+  <si>
+    <t>127_vhdl_call_vlog_Jedi</t>
   </si>
 </sst>
 </file>
@@ -2752,46 +2775,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="41" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="33" xfId="41" applyBorder="1" applyAlignment="1">
@@ -2799,6 +2806,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2815,17 +2825,30 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="41" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="41" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="44" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="41" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -5308,7 +5331,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{56F632E0-F7C1-4C1F-80EF-92B8CA0EC608}" diskRevisions="1" revisionId="733" version="13">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{8DF85B5D-CF7A-47B2-B954-AE8DB0AECDAD}" diskRevisions="1" revisionId="741" version="14">
   <header guid="{DB40D02A-1C38-451A-8E02-505A412F9BEE}" dateTime="2020-03-04T15:04:22" maxSheetId="5" userName="Jason Wang" r:id="rId1">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -5413,6 +5436,14 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{8DF85B5D-CF7A-47B2-B954-AE8DB0AECDAD}" dateTime="2020-03-09T16:24:32" maxSheetId="5" userName="Shawn Yan" r:id="rId14" minRId="734" maxRId="740">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -5467,6 +5498,92 @@
       </is>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="734" sId="2" xfDxf="1" dxf="1">
+    <nc r="C61" t="inlineStr">
+      <is>
+        <t>002_vhdl_combinat_adder8_Jedi</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <protection locked="0"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="735" sId="2" xfDxf="1" dxf="1">
+    <nc r="C62" t="inlineStr">
+      <is>
+        <t>007_vhdl_combinat_decoder2_Jedi</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <protection locked="0"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="736" sId="2" xfDxf="1" dxf="1">
+    <nc r="C63" t="inlineStr">
+      <is>
+        <t>013_vhdl_combinat_interupt_Jedi</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <protection locked="0"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="737" sId="2" xfDxf="1" dxf="1">
+    <nc r="C64" t="inlineStr">
+      <is>
+        <t>018_vhdl_combinat_tristate1_Jedi</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <protection locked="0"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="738" sId="2" xfDxf="1" dxf="1">
+    <nc r="C65" t="inlineStr">
+      <is>
+        <t>053_vhdl_sequentl_latches_Jedi</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <protection locked="0"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="739" sId="2" xfDxf="1" dxf="1">
+    <nc r="C66" t="inlineStr">
+      <is>
+        <t>067_vlog_combinat_alu_Jedi</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <protection locked="0"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="740" sId="2" xfDxf="1" dxf="1">
+    <nc r="C67" t="inlineStr">
+      <is>
+        <t>127_vhdl_call_vlog_Jedi</t>
+      </is>
+    </nc>
+    <ndxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <protection locked="0"/>
+    </ndxf>
+  </rcc>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_B9BD6881_07CB_45A2_88EA_37624FD6A1EC_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>case!$A$2:$AD$2</formula>
+  </rdn>
+  <rcv guid="{B9BD6881-07CB-45A2-88EA-37624FD6A1EC}" action="add"/>
 </revisions>
 </file>
 
@@ -11270,7 +11387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -11360,25 +11477,30 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
+    <customSheetView guid="{B9BD6881-07CB-45A2-88EA-37624FD6A1EC}">
+      <selection activeCell="B3" sqref="B3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B7" sqref="B7"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B7" sqref="B7"/>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -11386,12 +11508,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="A61" sqref="A61:XFD61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -12367,6 +12489,9 @@
       <c r="A61" s="18" t="s">
         <v>390</v>
       </c>
+      <c r="C61" s="18" t="s">
+        <v>400</v>
+      </c>
       <c r="D61" s="18" t="s">
         <v>272</v>
       </c>
@@ -12384,6 +12509,9 @@
       <c r="A62" s="18" t="s">
         <v>391</v>
       </c>
+      <c r="C62" s="18" t="s">
+        <v>401</v>
+      </c>
       <c r="D62" s="18" t="s">
         <v>272</v>
       </c>
@@ -12401,6 +12529,9 @@
       <c r="A63" s="18" t="s">
         <v>392</v>
       </c>
+      <c r="C63" s="18" t="s">
+        <v>402</v>
+      </c>
       <c r="D63" s="18" t="s">
         <v>272</v>
       </c>
@@ -12418,6 +12549,9 @@
       <c r="A64" s="18" t="s">
         <v>393</v>
       </c>
+      <c r="C64" s="18" t="s">
+        <v>403</v>
+      </c>
       <c r="D64" s="18" t="s">
         <v>272</v>
       </c>
@@ -12435,6 +12569,9 @@
       <c r="A65" s="18" t="s">
         <v>394</v>
       </c>
+      <c r="C65" s="18" t="s">
+        <v>404</v>
+      </c>
       <c r="D65" s="18" t="s">
         <v>272</v>
       </c>
@@ -12452,6 +12589,9 @@
       <c r="A66" s="18" t="s">
         <v>395</v>
       </c>
+      <c r="C66" s="18" t="s">
+        <v>405</v>
+      </c>
       <c r="D66" s="18" t="s">
         <v>309</v>
       </c>
@@ -12468,6 +12608,9 @@
     <row r="67" spans="1:19">
       <c r="A67" s="18" t="s">
         <v>396</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>406</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>331</v>
@@ -12486,26 +12629,33 @@
   <sheetProtection algorithmName="SHA-512" hashValue="4C55417S7/WEfM6p9p+2qxLa3pFuuwTQvkVS+xLflxPJ6JUMhmXb8UBi2EhWPKsWHpV7wPPZoM4Ci73L5pzjfA==" saltValue="OVPlytvnGy6tQU/SUgOtyg==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AD2"/>
   <customSheetViews>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+    <customSheetView guid="{B9BD6881-07CB-45A2-88EA-37624FD6A1EC}" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="A61" sqref="A61:XFD61"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:AD2"/>
+    </customSheetView>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <autoFilter ref="A2:AD2"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
       <autoFilter ref="A2:Y2"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" showAutoFilter="1">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-      <autoFilter ref="A2:AD2"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+      <autoFilter ref="A2:Y2"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -12522,7 +12672,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
@@ -12646,17 +12796,17 @@
       <c r="E109" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F109" s="73" t="s">
+      <c r="F109" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="G109" s="74"/>
-      <c r="H109" s="74"/>
-      <c r="I109" s="74"/>
-      <c r="J109" s="74"/>
-      <c r="K109" s="74"/>
-      <c r="L109" s="74"/>
-      <c r="M109" s="74"/>
-      <c r="N109" s="75"/>
+      <c r="G109" s="94"/>
+      <c r="H109" s="94"/>
+      <c r="I109" s="94"/>
+      <c r="J109" s="94"/>
+      <c r="K109" s="94"/>
+      <c r="L109" s="94"/>
+      <c r="M109" s="94"/>
+      <c r="N109" s="95"/>
     </row>
     <row r="110" spans="1:14">
       <c r="A110" s="6" t="s">
@@ -13494,7 +13644,7 @@
       <c r="A144" s="41">
         <v>1</v>
       </c>
-      <c r="B144" s="76" t="s">
+      <c r="B144" s="96" t="s">
         <v>122</v>
       </c>
       <c r="C144" s="39" t="s">
@@ -13520,7 +13670,7 @@
       <c r="A145" s="41">
         <v>2</v>
       </c>
-      <c r="B145" s="77"/>
+      <c r="B145" s="97"/>
       <c r="C145" s="39" t="s">
         <v>128</v>
       </c>
@@ -13542,7 +13692,7 @@
       <c r="A146" s="59">
         <v>3</v>
       </c>
-      <c r="B146" s="77"/>
+      <c r="B146" s="97"/>
       <c r="C146" s="39" t="s">
         <v>9</v>
       </c>
@@ -13560,7 +13710,7 @@
       <c r="A147" s="59">
         <v>4</v>
       </c>
-      <c r="B147" s="77"/>
+      <c r="B147" s="97"/>
       <c r="C147" s="60" t="s">
         <v>256</v>
       </c>
@@ -13582,7 +13732,7 @@
       <c r="A148" s="59">
         <v>5</v>
       </c>
-      <c r="B148" s="77"/>
+      <c r="B148" s="97"/>
       <c r="C148" s="39" t="s">
         <v>253</v>
       </c>
@@ -13602,7 +13752,7 @@
       <c r="A149" s="59">
         <v>6</v>
       </c>
-      <c r="B149" s="77"/>
+      <c r="B149" s="97"/>
       <c r="C149" s="60" t="s">
         <v>254</v>
       </c>
@@ -13624,7 +13774,7 @@
       <c r="A150" s="59">
         <v>7</v>
       </c>
-      <c r="B150" s="77"/>
+      <c r="B150" s="97"/>
       <c r="C150" s="39" t="s">
         <v>130</v>
       </c>
@@ -13646,7 +13796,7 @@
       <c r="A151" s="59">
         <v>8</v>
       </c>
-      <c r="B151" s="77"/>
+      <c r="B151" s="97"/>
       <c r="C151" s="39" t="s">
         <v>246</v>
       </c>
@@ -13668,7 +13818,7 @@
       <c r="A152" s="59">
         <v>9</v>
       </c>
-      <c r="B152" s="77"/>
+      <c r="B152" s="97"/>
       <c r="C152" s="39" t="s">
         <v>55</v>
       </c>
@@ -13692,7 +13842,7 @@
       <c r="A153" s="59">
         <v>10</v>
       </c>
-      <c r="B153" s="78"/>
+      <c r="B153" s="83"/>
       <c r="C153" s="39" t="s">
         <v>136</v>
       </c>
@@ -13714,7 +13864,7 @@
       <c r="A154" s="59">
         <v>11</v>
       </c>
-      <c r="B154" s="72" t="s">
+      <c r="B154" s="79" t="s">
         <v>139</v>
       </c>
       <c r="C154" s="39" t="s">
@@ -13740,7 +13890,7 @@
       <c r="A155" s="59">
         <v>12</v>
       </c>
-      <c r="B155" s="72"/>
+      <c r="B155" s="79"/>
       <c r="C155" s="39" t="s">
         <v>247</v>
       </c>
@@ -13764,7 +13914,7 @@
       <c r="A156" s="59">
         <v>13</v>
       </c>
-      <c r="B156" s="76" t="s">
+      <c r="B156" s="96" t="s">
         <v>143</v>
       </c>
       <c r="C156" s="39" t="s">
@@ -13788,7 +13938,7 @@
       <c r="A157" s="59">
         <v>14</v>
       </c>
-      <c r="B157" s="78"/>
+      <c r="B157" s="83"/>
       <c r="C157" s="39" t="s">
         <v>146</v>
       </c>
@@ -13808,7 +13958,7 @@
       <c r="A158" s="59">
         <v>15</v>
       </c>
-      <c r="B158" s="72" t="s">
+      <c r="B158" s="79" t="s">
         <v>148</v>
       </c>
       <c r="C158" s="39" t="s">
@@ -13832,7 +13982,7 @@
       <c r="A159" s="59">
         <v>16</v>
       </c>
-      <c r="B159" s="72"/>
+      <c r="B159" s="79"/>
       <c r="C159" s="39" t="s">
         <v>152</v>
       </c>
@@ -13852,7 +14002,7 @@
       <c r="A160" s="59">
         <v>17</v>
       </c>
-      <c r="B160" s="72"/>
+      <c r="B160" s="79"/>
       <c r="C160" s="39" t="s">
         <v>153</v>
       </c>
@@ -13872,7 +14022,7 @@
       <c r="A161" s="59">
         <v>18</v>
       </c>
-      <c r="B161" s="72"/>
+      <c r="B161" s="79"/>
       <c r="C161" s="39" t="s">
         <v>154</v>
       </c>
@@ -13892,7 +14042,7 @@
       <c r="A162" s="59">
         <v>19</v>
       </c>
-      <c r="B162" s="72"/>
+      <c r="B162" s="79"/>
       <c r="C162" s="39" t="s">
         <v>155</v>
       </c>
@@ -13912,7 +14062,7 @@
       <c r="A163" s="59">
         <v>20</v>
       </c>
-      <c r="B163" s="72"/>
+      <c r="B163" s="79"/>
       <c r="C163" s="39" t="s">
         <v>156</v>
       </c>
@@ -13932,7 +14082,7 @@
       <c r="A164" s="59">
         <v>21</v>
       </c>
-      <c r="B164" s="72"/>
+      <c r="B164" s="79"/>
       <c r="C164" s="39" t="s">
         <v>157</v>
       </c>
@@ -13952,7 +14102,7 @@
       <c r="A165" s="59">
         <v>22</v>
       </c>
-      <c r="B165" s="72"/>
+      <c r="B165" s="79"/>
       <c r="C165" s="39" t="s">
         <v>158</v>
       </c>
@@ -13972,7 +14122,7 @@
       <c r="A166" s="59">
         <v>23</v>
       </c>
-      <c r="B166" s="72" t="s">
+      <c r="B166" s="79" t="s">
         <v>159</v>
       </c>
       <c r="C166" s="39" t="s">
@@ -13996,7 +14146,7 @@
       <c r="A167" s="59">
         <v>24</v>
       </c>
-      <c r="B167" s="72"/>
+      <c r="B167" s="79"/>
       <c r="C167" s="39" t="s">
         <v>163</v>
       </c>
@@ -14018,7 +14168,7 @@
       <c r="A168" s="59">
         <v>25</v>
       </c>
-      <c r="B168" s="72"/>
+      <c r="B168" s="79"/>
       <c r="C168" s="39" t="s">
         <v>166</v>
       </c>
@@ -14040,7 +14190,7 @@
       <c r="A169" s="59">
         <v>26</v>
       </c>
-      <c r="B169" s="72" t="s">
+      <c r="B169" s="79" t="s">
         <v>169</v>
       </c>
       <c r="C169" s="39" t="s">
@@ -14064,7 +14214,7 @@
       <c r="A170" s="59">
         <v>27</v>
       </c>
-      <c r="B170" s="72"/>
+      <c r="B170" s="79"/>
       <c r="C170" s="39" t="s">
         <v>172</v>
       </c>
@@ -14086,7 +14236,7 @@
       <c r="A171" s="42">
         <v>28</v>
       </c>
-      <c r="B171" s="79"/>
+      <c r="B171" s="80"/>
       <c r="C171" s="40"/>
       <c r="D171" s="40"/>
       <c r="E171" s="40"/>
@@ -14122,11 +14272,11 @@
       <c r="B185" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="C185" s="80" t="s">
+      <c r="C185" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="D185" s="80"/>
-      <c r="E185" s="80"/>
+      <c r="D185" s="89"/>
+      <c r="E185" s="89"/>
       <c r="F185" s="34" t="s">
         <v>42</v>
       </c>
@@ -14135,17 +14285,17 @@
       </c>
     </row>
     <row r="186" spans="1:7">
-      <c r="A186" s="72" t="s">
+      <c r="A186" s="79" t="s">
         <v>180</v>
       </c>
-      <c r="B186" s="72" t="s">
+      <c r="B186" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="C186" s="81" t="s">
+      <c r="C186" s="90" t="s">
         <v>182</v>
       </c>
-      <c r="D186" s="81"/>
-      <c r="E186" s="81"/>
+      <c r="D186" s="90"/>
+      <c r="E186" s="90"/>
       <c r="F186" s="39" t="s">
         <v>183</v>
       </c>
@@ -14154,13 +14304,13 @@
       </c>
     </row>
     <row r="187" spans="1:7">
-      <c r="A187" s="72"/>
-      <c r="B187" s="72"/>
-      <c r="C187" s="82" t="s">
+      <c r="A187" s="79"/>
+      <c r="B187" s="79"/>
+      <c r="C187" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="D187" s="82"/>
-      <c r="E187" s="82"/>
+      <c r="D187" s="91"/>
+      <c r="E187" s="91"/>
       <c r="F187" s="39" t="s">
         <v>185</v>
       </c>
@@ -14169,15 +14319,15 @@
       </c>
     </row>
     <row r="188" spans="1:7">
-      <c r="A188" s="72"/>
-      <c r="B188" s="72" t="s">
+      <c r="A188" s="79"/>
+      <c r="B188" s="79" t="s">
         <v>186</v>
       </c>
-      <c r="C188" s="83" t="s">
+      <c r="C188" s="92" t="s">
         <v>187</v>
       </c>
-      <c r="D188" s="83"/>
-      <c r="E188" s="83"/>
+      <c r="D188" s="92"/>
+      <c r="E188" s="92"/>
       <c r="F188" s="39" t="s">
         <v>183</v>
       </c>
@@ -14186,13 +14336,13 @@
       </c>
     </row>
     <row r="189" spans="1:7">
-      <c r="A189" s="72"/>
-      <c r="B189" s="72"/>
-      <c r="C189" s="83" t="s">
+      <c r="A189" s="79"/>
+      <c r="B189" s="79"/>
+      <c r="C189" s="92" t="s">
         <v>187</v>
       </c>
-      <c r="D189" s="83"/>
-      <c r="E189" s="83"/>
+      <c r="D189" s="92"/>
+      <c r="E189" s="92"/>
       <c r="F189" s="39" t="s">
         <v>185</v>
       </c>
@@ -14201,17 +14351,17 @@
       </c>
     </row>
     <row r="190" spans="1:7">
-      <c r="A190" s="84" t="s">
+      <c r="A190" s="77" t="s">
         <v>188</v>
       </c>
-      <c r="B190" s="72" t="s">
+      <c r="B190" s="79" t="s">
         <v>189</v>
       </c>
-      <c r="C190" s="72" t="s">
+      <c r="C190" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="D190" s="72"/>
-      <c r="E190" s="72"/>
+      <c r="D190" s="79"/>
+      <c r="E190" s="79"/>
       <c r="F190" s="39" t="s">
         <v>183</v>
       </c>
@@ -14220,13 +14370,13 @@
       </c>
     </row>
     <row r="191" spans="1:7">
-      <c r="A191" s="84"/>
-      <c r="B191" s="72"/>
-      <c r="C191" s="72" t="s">
+      <c r="A191" s="77"/>
+      <c r="B191" s="79"/>
+      <c r="C191" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="D191" s="72"/>
-      <c r="E191" s="72"/>
+      <c r="D191" s="79"/>
+      <c r="E191" s="79"/>
       <c r="F191" s="39" t="s">
         <v>185</v>
       </c>
@@ -14235,15 +14385,15 @@
       </c>
     </row>
     <row r="192" spans="1:7">
-      <c r="A192" s="84"/>
-      <c r="B192" s="72" t="s">
+      <c r="A192" s="77"/>
+      <c r="B192" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="C192" s="72" t="s">
+      <c r="C192" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="D192" s="72"/>
-      <c r="E192" s="72"/>
+      <c r="D192" s="79"/>
+      <c r="E192" s="79"/>
       <c r="F192" s="39" t="s">
         <v>183</v>
       </c>
@@ -14252,13 +14402,13 @@
       </c>
     </row>
     <row r="193" spans="1:7">
-      <c r="A193" s="84"/>
-      <c r="B193" s="72"/>
-      <c r="C193" s="72" t="s">
+      <c r="A193" s="77"/>
+      <c r="B193" s="79"/>
+      <c r="C193" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="D193" s="72"/>
-      <c r="E193" s="72"/>
+      <c r="D193" s="79"/>
+      <c r="E193" s="79"/>
       <c r="F193" s="39" t="s">
         <v>185</v>
       </c>
@@ -14267,17 +14417,17 @@
       </c>
     </row>
     <row r="194" spans="1:7">
-      <c r="A194" s="84" t="s">
+      <c r="A194" s="77" t="s">
         <v>191</v>
       </c>
-      <c r="B194" s="72" t="s">
+      <c r="B194" s="79" t="s">
         <v>192</v>
       </c>
-      <c r="C194" s="72" t="s">
+      <c r="C194" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="D194" s="72"/>
-      <c r="E194" s="72"/>
+      <c r="D194" s="79"/>
+      <c r="E194" s="79"/>
       <c r="F194" s="39" t="s">
         <v>183</v>
       </c>
@@ -14286,13 +14436,13 @@
       </c>
     </row>
     <row r="195" spans="1:7">
-      <c r="A195" s="84"/>
-      <c r="B195" s="72"/>
-      <c r="C195" s="72" t="s">
+      <c r="A195" s="77"/>
+      <c r="B195" s="79"/>
+      <c r="C195" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="D195" s="72"/>
-      <c r="E195" s="72"/>
+      <c r="D195" s="79"/>
+      <c r="E195" s="79"/>
       <c r="F195" s="39" t="s">
         <v>185</v>
       </c>
@@ -14301,15 +14451,15 @@
       </c>
     </row>
     <row r="196" spans="1:7">
-      <c r="A196" s="84"/>
-      <c r="B196" s="72" t="s">
+      <c r="A196" s="77"/>
+      <c r="B196" s="79" t="s">
         <v>193</v>
       </c>
-      <c r="C196" s="72" t="s">
+      <c r="C196" s="79" t="s">
         <v>194</v>
       </c>
-      <c r="D196" s="72"/>
-      <c r="E196" s="72"/>
+      <c r="D196" s="79"/>
+      <c r="E196" s="79"/>
       <c r="F196" s="39" t="s">
         <v>183</v>
       </c>
@@ -14318,13 +14468,13 @@
       </c>
     </row>
     <row r="197" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A197" s="86"/>
-      <c r="B197" s="79"/>
-      <c r="C197" s="79" t="s">
+      <c r="A197" s="78"/>
+      <c r="B197" s="80"/>
+      <c r="C197" s="80" t="s">
         <v>195</v>
       </c>
-      <c r="D197" s="79"/>
-      <c r="E197" s="79"/>
+      <c r="D197" s="80"/>
+      <c r="E197" s="80"/>
       <c r="F197" s="40" t="s">
         <v>185</v>
       </c>
@@ -14363,12 +14513,12 @@
       <c r="A202" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="B202" s="87" t="s">
+      <c r="B202" s="81" t="s">
         <v>198</v>
       </c>
-      <c r="C202" s="87"/>
-      <c r="D202" s="87"/>
-      <c r="E202" s="87"/>
+      <c r="C202" s="81"/>
+      <c r="D202" s="81"/>
+      <c r="E202" s="81"/>
       <c r="F202" s="22" t="s">
         <v>199</v>
       </c>
@@ -14380,12 +14530,12 @@
       <c r="A203" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="B203" s="88" t="s">
+      <c r="B203" s="82" t="s">
         <v>202</v>
       </c>
-      <c r="C203" s="78"/>
-      <c r="D203" s="78"/>
-      <c r="E203" s="78"/>
+      <c r="C203" s="83"/>
+      <c r="D203" s="83"/>
+      <c r="E203" s="83"/>
       <c r="F203" s="36" t="s">
         <v>203</v>
       </c>
@@ -14397,12 +14547,12 @@
       <c r="A204" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="B204" s="89" t="s">
+      <c r="B204" s="84" t="s">
         <v>205</v>
       </c>
-      <c r="C204" s="90"/>
-      <c r="D204" s="90"/>
-      <c r="E204" s="91"/>
+      <c r="C204" s="85"/>
+      <c r="D204" s="85"/>
+      <c r="E204" s="86"/>
       <c r="F204" s="10" t="s">
         <v>184</v>
       </c>
@@ -14414,12 +14564,12 @@
       <c r="A205" s="45" t="s">
         <v>230</v>
       </c>
-      <c r="B205" s="89" t="s">
+      <c r="B205" s="84" t="s">
         <v>233</v>
       </c>
-      <c r="C205" s="90"/>
-      <c r="D205" s="90"/>
-      <c r="E205" s="91"/>
+      <c r="C205" s="85"/>
+      <c r="D205" s="85"/>
+      <c r="E205" s="86"/>
       <c r="F205" s="46" t="s">
         <v>231</v>
       </c>
@@ -14431,12 +14581,12 @@
       <c r="A206" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="B206" s="92" t="s">
+      <c r="B206" s="87" t="s">
         <v>234</v>
       </c>
-      <c r="C206" s="79"/>
-      <c r="D206" s="79"/>
-      <c r="E206" s="79"/>
+      <c r="C206" s="80"/>
+      <c r="D206" s="80"/>
+      <c r="E206" s="80"/>
       <c r="F206" s="13" t="s">
         <v>184</v>
       </c>
@@ -14481,11 +14631,11 @@
       <c r="C211" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D211" s="93" t="s">
+      <c r="D211" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="E211" s="93"/>
-      <c r="F211" s="93"/>
+      <c r="E211" s="88"/>
+      <c r="F211" s="88"/>
       <c r="G211" s="32"/>
     </row>
     <row r="212" spans="1:7">
@@ -14498,11 +14648,11 @@
       <c r="C212" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D212" s="85" t="s">
+      <c r="D212" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="E212" s="85"/>
-      <c r="F212" s="85"/>
+      <c r="E212" s="72"/>
+      <c r="F212" s="72"/>
       <c r="G212" s="24"/>
     </row>
     <row r="213" spans="1:7">
@@ -14515,11 +14665,11 @@
       <c r="C213" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D213" s="85" t="s">
+      <c r="D213" s="72" t="s">
         <v>209</v>
       </c>
-      <c r="E213" s="85"/>
-      <c r="F213" s="85"/>
+      <c r="E213" s="72"/>
+      <c r="F213" s="72"/>
       <c r="G213" s="24"/>
     </row>
     <row r="214" spans="1:7">
@@ -14532,11 +14682,11 @@
       <c r="C214" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="D214" s="85" t="s">
+      <c r="D214" s="72" t="s">
         <v>211</v>
       </c>
-      <c r="E214" s="85"/>
-      <c r="F214" s="85"/>
+      <c r="E214" s="72"/>
+      <c r="F214" s="72"/>
       <c r="G214" s="24"/>
     </row>
     <row r="215" spans="1:7">
@@ -14549,11 +14699,11 @@
       <c r="C215" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="D215" s="85" t="s">
+      <c r="D215" s="72" t="s">
         <v>222</v>
       </c>
-      <c r="E215" s="85"/>
-      <c r="F215" s="85"/>
+      <c r="E215" s="72"/>
+      <c r="F215" s="72"/>
       <c r="G215" s="24"/>
     </row>
     <row r="216" spans="1:7">
@@ -14566,11 +14716,11 @@
       <c r="C216" s="39" t="s">
         <v>236</v>
       </c>
-      <c r="D216" s="85" t="s">
+      <c r="D216" s="72" t="s">
         <v>235</v>
       </c>
-      <c r="E216" s="85"/>
-      <c r="F216" s="85"/>
+      <c r="E216" s="72"/>
+      <c r="F216" s="72"/>
       <c r="G216" s="24"/>
     </row>
     <row r="217" spans="1:7">
@@ -14583,11 +14733,11 @@
       <c r="C217" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D217" s="95" t="s">
+      <c r="D217" s="74" t="s">
         <v>237</v>
       </c>
-      <c r="E217" s="96"/>
-      <c r="F217" s="97"/>
+      <c r="E217" s="75"/>
+      <c r="F217" s="76"/>
       <c r="G217" s="53"/>
     </row>
     <row r="218" spans="1:7">
@@ -14600,11 +14750,11 @@
       <c r="C218" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="D218" s="95" t="s">
+      <c r="D218" s="74" t="s">
         <v>238</v>
       </c>
-      <c r="E218" s="96"/>
-      <c r="F218" s="97"/>
+      <c r="E218" s="75"/>
+      <c r="F218" s="76"/>
       <c r="G218" s="53"/>
     </row>
     <row r="219" spans="1:7">
@@ -14617,11 +14767,11 @@
       <c r="C219" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D219" s="95" t="s">
+      <c r="D219" s="74" t="s">
         <v>251</v>
       </c>
-      <c r="E219" s="96"/>
-      <c r="F219" s="97"/>
+      <c r="E219" s="75"/>
+      <c r="F219" s="76"/>
       <c r="G219" s="53"/>
     </row>
     <row r="220" spans="1:7">
@@ -14668,31 +14818,50 @@
       <c r="C222" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D222" s="94" t="s">
+      <c r="D222" s="73" t="s">
         <v>264</v>
       </c>
-      <c r="E222" s="94"/>
-      <c r="F222" s="94"/>
+      <c r="E222" s="73"/>
+      <c r="F222" s="73"/>
       <c r="G222" s="25"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ZC0B/yWBsnsNoiYGsylBtDFjHlFkDcsc5FbUMdgfxj9Hei+XekJLxNRsfmgfru30ZY2RAy7fdFIuraUAtim1lw==" saltValue="HBb3PLugL4bod/dSynZVew==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{B9BD6881-07CB-45A2-88EA-37624FD6A1EC}" scale="115">
       <selection activeCell="D224" sqref="D224"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+      <selection activeCell="D224" sqref="D224"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+    </customSheetView>
   </customSheetViews>
   <mergeCells count="44">
-    <mergeCell ref="D213:F213"/>
-    <mergeCell ref="D214:F214"/>
-    <mergeCell ref="D215:F215"/>
-    <mergeCell ref="D216:F216"/>
-    <mergeCell ref="D222:F222"/>
-    <mergeCell ref="D217:F217"/>
-    <mergeCell ref="D218:F218"/>
-    <mergeCell ref="D219:F219"/>
+    <mergeCell ref="B166:B168"/>
+    <mergeCell ref="F109:N109"/>
+    <mergeCell ref="B144:B153"/>
+    <mergeCell ref="B154:B155"/>
+    <mergeCell ref="B156:B157"/>
+    <mergeCell ref="B158:B165"/>
+    <mergeCell ref="B169:B171"/>
+    <mergeCell ref="C185:E185"/>
+    <mergeCell ref="A186:A189"/>
+    <mergeCell ref="B186:B187"/>
+    <mergeCell ref="C186:E186"/>
+    <mergeCell ref="C187:E187"/>
+    <mergeCell ref="B188:B189"/>
+    <mergeCell ref="C188:E188"/>
+    <mergeCell ref="C189:E189"/>
+    <mergeCell ref="A190:A193"/>
+    <mergeCell ref="B190:B191"/>
+    <mergeCell ref="C190:E190"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="B192:B193"/>
+    <mergeCell ref="C192:E192"/>
+    <mergeCell ref="C193:E193"/>
     <mergeCell ref="D212:F212"/>
     <mergeCell ref="A194:A197"/>
     <mergeCell ref="B194:B195"/>
@@ -14707,33 +14876,19 @@
     <mergeCell ref="B206:E206"/>
     <mergeCell ref="D211:F211"/>
     <mergeCell ref="B205:E205"/>
-    <mergeCell ref="A190:A193"/>
-    <mergeCell ref="B190:B191"/>
-    <mergeCell ref="C190:E190"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="B192:B193"/>
-    <mergeCell ref="C192:E192"/>
-    <mergeCell ref="C193:E193"/>
-    <mergeCell ref="B169:B171"/>
-    <mergeCell ref="C185:E185"/>
-    <mergeCell ref="A186:A189"/>
-    <mergeCell ref="B186:B187"/>
-    <mergeCell ref="C186:E186"/>
-    <mergeCell ref="C187:E187"/>
-    <mergeCell ref="B188:B189"/>
-    <mergeCell ref="C188:E188"/>
-    <mergeCell ref="C189:E189"/>
-    <mergeCell ref="B166:B168"/>
-    <mergeCell ref="F109:N109"/>
-    <mergeCell ref="B144:B153"/>
-    <mergeCell ref="B154:B155"/>
-    <mergeCell ref="B156:B157"/>
-    <mergeCell ref="B158:B165"/>
+    <mergeCell ref="D213:F213"/>
+    <mergeCell ref="D214:F214"/>
+    <mergeCell ref="D215:F215"/>
+    <mergeCell ref="D216:F216"/>
+    <mergeCell ref="D222:F222"/>
+    <mergeCell ref="D217:F217"/>
+    <mergeCell ref="D218:F218"/>
+    <mergeCell ref="D219:F219"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -14752,15 +14907,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{B9BD6881-07CB-45A2-88EA-37624FD6A1EC}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>